<commit_message>
feat: model name filter
</commit_message>
<xml_diff>
--- a/results/history.xlsx
+++ b/results/history.xlsx
@@ -77,7 +77,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -94,6 +94,7 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -459,12 +460,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
@@ -481,6 +486,8 @@
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -509,6 +516,16 @@
           <t>2025-12-14 17:12:45</t>
         </is>
       </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-14 19:36:19</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-14 19:41:18</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -536,6 +553,7 @@
           <t>OK (1944ms)</t>
         </is>
       </c>
+      <c r="F2" s="6" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -563,6 +581,7 @@
           <t>429</t>
         </is>
       </c>
+      <c r="F3" s="6" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -590,6 +609,7 @@
           <t>OK (8973ms)</t>
         </is>
       </c>
+      <c r="F4" s="6" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -617,6 +637,7 @@
           <t>OK (831ms)</t>
         </is>
       </c>
+      <c r="F5" s="6" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -644,6 +665,16 @@
           <t>429</t>
         </is>
       </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>OK (1584ms)</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>OK (1257ms)</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -671,6 +702,16 @@
           <t>OK (2337ms)</t>
         </is>
       </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>429</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>429</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -698,6 +739,16 @@
           <t>OK (3852ms)</t>
         </is>
       </c>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>OK (2903ms)</t>
+        </is>
+      </c>
+      <c r="G8" s="4" t="inlineStr">
+        <is>
+          <t>OK (5822ms)</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
@@ -725,6 +776,16 @@
           <t>OK (1388ms)</t>
         </is>
       </c>
+      <c r="F9" s="4" t="inlineStr">
+        <is>
+          <t>OK (1472ms)</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>OK (1501ms)</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
@@ -752,6 +813,16 @@
           <t>OK (1480ms)</t>
         </is>
       </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t>OK (1663ms)</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>OK (1286ms)</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
@@ -777,6 +848,100 @@
       <c r="E11" s="4" t="inlineStr">
         <is>
           <t>OK (1067ms)</t>
+        </is>
+      </c>
+      <c r="F11" s="4" t="inlineStr">
+        <is>
+          <t>OK (1242ms)</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>OK (1282ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>google/gemma-3n-e4b-it:free</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="n"/>
+      <c r="C12" s="6" t="n"/>
+      <c r="D12" s="6" t="n"/>
+      <c r="E12" s="6" t="n"/>
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>OK (1266ms)</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>OK (1485ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>mistralai/devstral-2512:free</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="n"/>
+      <c r="C13" s="6" t="n"/>
+      <c r="D13" s="6" t="n"/>
+      <c r="E13" s="6" t="n"/>
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>OK (3733ms)</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="inlineStr">
+        <is>
+          <t>429</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>mistralai/mistral-7b-instruct:free</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="n"/>
+      <c r="C14" s="6" t="n"/>
+      <c r="D14" s="6" t="n"/>
+      <c r="E14" s="6" t="n"/>
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>OK (692ms)</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>OK (1290ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>mistralai/mistral-small-3.1-24b-instruct:free</t>
+        </is>
+      </c>
+      <c r="B15" s="6" t="n"/>
+      <c r="C15" s="6" t="n"/>
+      <c r="D15" s="6" t="n"/>
+      <c r="E15" s="6" t="n"/>
+      <c r="F15" s="4" t="inlineStr">
+        <is>
+          <t>OK (1418ms)</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="inlineStr">
+        <is>
+          <t>OK (937ms)</t>
         </is>
       </c>
     </row>

</xml_diff>